<commit_message>
bug in indexing the impact assessment
</commit_message>
<xml_diff>
--- a/CIVICS_Ghana/IO_Ghana/Pumpfed Irrigation for Maize/Baseline Results/Pumpfed Irrigation for Maize - baseline.xlsx
+++ b/CIVICS_Ghana/IO_Ghana/Pumpfed Irrigation for Maize/Baseline Results/Pumpfed Irrigation for Maize - baseline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Investment</t>
   </si>
@@ -80,6 +80,24 @@
   </si>
   <si>
     <t>Capital Total Impact</t>
+  </si>
+  <si>
+    <t>M GHS</t>
+  </si>
+  <si>
+    <t>1/years</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>Mm3</t>
+  </si>
+  <si>
+    <t>kton</t>
+  </si>
+  <si>
+    <t>kha</t>
   </si>
   <si>
     <t>Pumpfed Irrigation for Maize</t>
@@ -443,13 +461,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:24">
+      <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,76 +537,145 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C2">
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
         <v>125.8672760472691</v>
       </c>
-      <c r="D2">
+      <c r="D4">
         <v>715.2023191869084</v>
       </c>
-      <c r="E2">
+      <c r="E4">
         <v>5.682194305359529</v>
       </c>
-      <c r="F2">
+      <c r="F4">
         <v>0.1759883499683891</v>
       </c>
-      <c r="G2">
-        <v>7.600832898460794</v>
-      </c>
-      <c r="H2">
-        <v>0.7923669199008145</v>
-      </c>
-      <c r="I2">
-        <v>337.3223714462074</v>
-      </c>
-      <c r="J2">
+      <c r="G4">
+        <v>7.192313248880737</v>
+      </c>
+      <c r="H4">
+        <v>33.94489230068575</v>
+      </c>
+      <c r="I4">
+        <v>337.0500250131554</v>
+      </c>
+      <c r="J4">
         <v>39.66921853806707</v>
       </c>
-      <c r="K2">
+      <c r="K4">
         <v>377.7461571722815</v>
       </c>
-      <c r="L2">
+      <c r="L4">
         <v>270.477081390447</v>
       </c>
-      <c r="M2">
-        <v>0.007521533916587941</v>
-      </c>
-      <c r="N2">
-        <v>1.343500960498204</v>
-      </c>
-      <c r="O2">
-        <v>0.007235826866235584</v>
-      </c>
-      <c r="P2">
+      <c r="M4">
+        <v>0.002309998559894666</v>
+      </c>
+      <c r="N4">
+        <v>15.77667327413656</v>
+      </c>
+      <c r="O4">
+        <v>0.003761469974051579</v>
+      </c>
+      <c r="P4">
         <v>102.3345925394533</v>
       </c>
-      <c r="Q2">
+      <c r="Q4">
         <v>0.06649889930849895</v>
       </c>
-      <c r="R2">
+      <c r="R4">
         <v>0.3105979636602569</v>
       </c>
-      <c r="S2">
-        <v>-76.00080745069135</v>
-      </c>
-      <c r="T2">
-        <v>-6.580168238509941</v>
-      </c>
-      <c r="U2">
-        <v>-3373.216478635208</v>
-      </c>
-      <c r="V2">
+      <c r="S4">
+        <v>-71.92082249024747</v>
+      </c>
+      <c r="T4">
+        <v>-323.672249732721</v>
+      </c>
+      <c r="U4">
+        <v>-3370.49648866158</v>
+      </c>
+      <c r="V4">
         <v>-294.3575928412174</v>
       </c>
-      <c r="W2">
+      <c r="W4">
         <v>-2704.704315005161</v>
       </c>
-      <c r="X2">
+      <c r="X4">
         <v>-3777.150973759155</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CIVICS Ghana Shock1 done!
</commit_message>
<xml_diff>
--- a/CIVICS_Ghana/IO_Ghana/Pumpfed Irrigation for Maize/Baseline Results/Pumpfed Irrigation for Maize - baseline.xlsx
+++ b/CIVICS_Ghana/IO_Ghana/Pumpfed Irrigation for Maize/Baseline Results/Pumpfed Irrigation for Maize - baseline.xlsx
@@ -613,25 +613,25 @@
         <v>29</v>
       </c>
       <c r="C4">
-        <v>125.8672760472691</v>
+        <v>142.4651586029795</v>
       </c>
       <c r="D4">
         <v>715.2023191869084</v>
       </c>
       <c r="E4">
-        <v>5.682194305359529</v>
+        <v>5.020191085316707</v>
       </c>
       <c r="F4">
-        <v>0.1759883499683891</v>
+        <v>0.1991956049093126</v>
       </c>
       <c r="G4">
-        <v>7.192313248880737</v>
+        <v>-325.3792547059857</v>
       </c>
       <c r="H4">
-        <v>33.94489230068575</v>
+        <v>11775.03710062947</v>
       </c>
       <c r="I4">
-        <v>337.0500250131554</v>
+        <v>158.8643429998319</v>
       </c>
       <c r="J4">
         <v>39.66921853806707</v>
@@ -643,40 +643,40 @@
         <v>270.477081390447</v>
       </c>
       <c r="M4">
-        <v>0.002309998559894666</v>
+        <v>0.1404877219320042</v>
       </c>
       <c r="N4">
-        <v>15.77667327413656</v>
+        <v>11.85561165795662</v>
       </c>
       <c r="O4">
-        <v>0.003761469974051579</v>
+        <v>0.002006714086746797</v>
       </c>
       <c r="P4">
-        <v>102.3345925394533</v>
+        <v>115.829264083106</v>
       </c>
       <c r="Q4">
-        <v>0.06649889930849895</v>
+        <v>0.07526798493927345</v>
       </c>
       <c r="R4">
-        <v>0.3105979636602569</v>
+        <v>0.351555936911609</v>
       </c>
       <c r="S4">
-        <v>-71.92082249024747</v>
+        <v>3253.933034781789</v>
       </c>
       <c r="T4">
-        <v>-323.672249732721</v>
+        <v>-117738.5153946368</v>
       </c>
       <c r="U4">
-        <v>-3370.49648866158</v>
+        <v>-1588.641423284233</v>
       </c>
       <c r="V4">
-        <v>-294.3575928412174</v>
+        <v>-280.8629212975648</v>
       </c>
       <c r="W4">
-        <v>-2704.704315005161</v>
+        <v>-2704.695545919531</v>
       </c>
       <c r="X4">
-        <v>-3777.150973759155</v>
+        <v>-3777.110015785904</v>
       </c>
     </row>
   </sheetData>

</xml_diff>